<commit_message>
mul uint64 uint64 -> uint96
</commit_message>
<xml_diff>
--- a/AsmInt64Mul.xlsx
+++ b/AsmInt64Mul.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="8730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="8730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>2 * 4-stellige Zahlen</t>
   </si>
@@ -42,6 +43,18 @@
   </si>
   <si>
     <t>Jeder Kasten entspricht 64-Bit:</t>
+  </si>
+  <si>
+    <t>[esp+4]</t>
+  </si>
+  <si>
+    <t>[esp+8]</t>
+  </si>
+  <si>
+    <t>[esp+12]</t>
+  </si>
+  <si>
+    <t>[esp+16]</t>
   </si>
 </sst>
 </file>
@@ -73,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -142,11 +155,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -160,6 +184,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -442,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,4 +626,198 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>5584</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>4927</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8">
+        <f>B3*D3</f>
+        <v>27512368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <f>(B3-E9)/100</f>
+        <v>55</v>
+      </c>
+      <c r="E9" s="2">
+        <f>MOD(B3, 100)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f>(D9*100+E9)*(D13*100+E13)</f>
+        <v>27512368</v>
+      </c>
+      <c r="G11" t="str">
+        <f>IF(F11=F3, "OK", "Achtung")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <f>(D3-E13)/100</f>
+        <v>49</v>
+      </c>
+      <c r="E13" s="2">
+        <f>MOD(D3, 100)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <f>(D13*D9-C16)/100</f>
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
+        <f>MOD(D13*D9,100)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <f>(D9*E13-D18)/100</f>
+        <v>14</v>
+      </c>
+      <c r="D18" s="2">
+        <f>MOD(D9*E13,100)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <f>(D13*E9-D19)/100</f>
+        <v>41</v>
+      </c>
+      <c r="D19" s="2">
+        <f>MOD(D13*E9,100)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D20" s="10">
+        <f>(E9*E13 - E20)/100</f>
+        <v>22</v>
+      </c>
+      <c r="E20" s="2">
+        <f>MOD(E9*E13, 100)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <f>(SUM(C16:C21)-C23)/100</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <f>(SUM(D16:D21)-D23)/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>SUM(B16:B21)</f>
+        <v>27</v>
+      </c>
+      <c r="C23">
+        <f>MOD(SUM(C16:C21), 100)</f>
+        <v>51</v>
+      </c>
+      <c r="D23">
+        <f>MOD(SUM(D16:D21), 100)</f>
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <f>E20</f>
+        <v>68</v>
+      </c>
+      <c r="F23">
+        <f>(B23*1000000) + (C23* 10000) + (D23*100) + E23</f>
+        <v>27512368</v>
+      </c>
+      <c r="G23" t="str">
+        <f>IF(F23=F11, "OK", "Achtung")</f>
+        <v>OK</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>